<commit_message>
Mixture Prediction Results(Master / Target / GAN / Real)
</commit_message>
<xml_diff>
--- a/Mixture Prediction Results.xlsx
+++ b/Mixture Prediction Results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\study_data\problem\模型迁移\github-model-transfer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\study_data\problem\模型迁移\github-model-transfer\Raman-model-transfer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{887F210A-0258-48B6-AD06-DF2F756BB139}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B80DD30E-F294-4F4B-8633-81C486AC9750}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="1185" yWindow="1830" windowWidth="17460" windowHeight="11370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mixture Prediction Results" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="76">
   <si>
     <t>10_乙醇-正丙醇#2-3_1</t>
   </si>
@@ -229,11 +229,35 @@
     <t>Real labels</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
+  <si>
+    <t>acetonitrile</t>
+  </si>
+  <si>
+    <t>ethanol</t>
+  </si>
+  <si>
+    <t>glutaraldehyde</t>
+  </si>
+  <si>
+    <t>propanol</t>
+  </si>
+  <si>
+    <t>pentanol</t>
+  </si>
+  <si>
+    <t>tetraethyl orthosilicate</t>
+  </si>
+  <si>
+    <t>cyclohexane</t>
+  </si>
+  <si>
+    <t>methanol</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1190,10 +1214,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BE39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:BE48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -7425,8 +7451,73 @@
         <v>1</v>
       </c>
     </row>
+    <row r="41" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>56</v>
+      </c>
+      <c r="B41" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="42" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>57</v>
+      </c>
+      <c r="B42" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="43" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>58</v>
+      </c>
+      <c r="B43" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="44" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>59</v>
+      </c>
+      <c r="B44" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="45" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>60</v>
+      </c>
+      <c r="B45" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="46" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>61</v>
+      </c>
+      <c r="B46" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="47" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>62</v>
+      </c>
+      <c r="B47" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="48" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>63</v>
+      </c>
+      <c r="B48" t="s">
+        <v>75</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>